<commit_message>
Perbaikan use case dan sedikit
</commit_message>
<xml_diff>
--- a/New Microsoft Excel Worksheet.xlsx
+++ b/New Microsoft Excel Worksheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="115">
   <si>
     <t>Pilih Citra</t>
   </si>
@@ -345,6 +345,21 @@
   </si>
   <si>
     <t>1. Mengubah nilai parameter c1, c2 atau centang seluruh nilai c1 dan seluruh nilai c2</t>
+  </si>
+  <si>
+    <t>Tampilkan Data Fisik</t>
+  </si>
+  <si>
+    <t>User membuka form Tampil untuk melihat data fisik citra awal dan hasil</t>
+  </si>
+  <si>
+    <t>User telah membuka form Tampil</t>
+  </si>
+  <si>
+    <t>1. Memilih tombol Tampil</t>
+  </si>
+  <si>
+    <t>2. Menampilkan tabel data fisik untuk citra awal, AFCEDP, dan ACEDP</t>
   </si>
 </sst>
 </file>
@@ -512,56 +527,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -575,12 +551,54 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -589,9 +607,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -915,91 +930,91 @@
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="16"/>
+      <c r="C2" s="32"/>
       <c r="E2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="16" t="s">
+      <c r="F2" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="G2" s="16"/>
+      <c r="G2" s="32"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="16"/>
+      <c r="B3" s="32" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="32"/>
       <c r="E3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="G3" s="16"/>
+      <c r="F3" s="32" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" s="32"/>
     </row>
     <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="16"/>
+      <c r="C4" s="32"/>
       <c r="E4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="16" t="s">
+      <c r="F4" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="G4" s="16"/>
+      <c r="G4" s="32"/>
     </row>
     <row r="5" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="16"/>
+      <c r="C5" s="32"/>
       <c r="E5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="16" t="s">
+      <c r="F5" s="32" t="s">
         <v>16</v>
       </c>
-      <c r="G5" s="16"/>
+      <c r="G5" s="32"/>
     </row>
     <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="16"/>
+      <c r="C6" s="32"/>
       <c r="E6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="16" t="s">
+      <c r="F6" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="G6" s="16"/>
+      <c r="G6" s="32"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="19"/>
+      <c r="A7" s="31"/>
       <c r="B7" s="4" t="s">
         <v>6</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="20"/>
+      <c r="E7" s="35"/>
       <c r="F7" s="4" t="s">
         <v>6</v>
       </c>
@@ -1008,14 +1023,14 @@
       </c>
     </row>
     <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="19"/>
+      <c r="A8" s="31"/>
       <c r="B8" s="10" t="s">
         <v>9</v>
       </c>
       <c r="C8" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="21"/>
+      <c r="E8" s="37"/>
       <c r="F8" s="2" t="s">
         <v>46</v>
       </c>
@@ -1024,21 +1039,21 @@
       </c>
     </row>
     <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="19"/>
+      <c r="A9" s="31"/>
       <c r="B9" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E9" s="21"/>
+      <c r="E9" s="37"/>
       <c r="F9" s="2"/>
       <c r="G9" s="2" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="E10" s="21"/>
+      <c r="E10" s="37"/>
       <c r="F10" s="1"/>
       <c r="G10" s="2" t="s">
         <v>50</v>
@@ -1048,11 +1063,11 @@
       <c r="A11" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B11" s="17" t="s">
+      <c r="B11" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="18"/>
-      <c r="E11" s="22"/>
+      <c r="C11" s="34"/>
+      <c r="E11" s="36"/>
       <c r="F11" s="1"/>
       <c r="G11" s="2" t="s">
         <v>51</v>
@@ -1062,10 +1077,10 @@
       <c r="A12" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B12" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="C12" s="18"/>
+      <c r="B12" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="34"/>
       <c r="E12" s="7"/>
       <c r="F12" s="11"/>
       <c r="G12" s="11"/>
@@ -1074,52 +1089,52 @@
       <c r="A13" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="17" t="s">
+      <c r="B13" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="18"/>
+      <c r="C13" s="34"/>
       <c r="E13" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F13" s="16" t="s">
+      <c r="F13" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="G13" s="16"/>
+      <c r="G13" s="32"/>
     </row>
     <row r="14" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B14" s="17" t="s">
+      <c r="B14" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="18"/>
+      <c r="C14" s="34"/>
       <c r="E14" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F14" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="G14" s="16"/>
+      <c r="F14" s="32" t="s">
+        <v>6</v>
+      </c>
+      <c r="G14" s="32"/>
     </row>
     <row r="15" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B15" s="17" t="s">
+      <c r="B15" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="18"/>
+      <c r="C15" s="34"/>
       <c r="E15" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F15" s="16" t="s">
+      <c r="F15" s="32" t="s">
         <v>53</v>
       </c>
-      <c r="G15" s="16"/>
+      <c r="G15" s="32"/>
     </row>
     <row r="16" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="19"/>
+      <c r="A16" s="31"/>
       <c r="B16" s="4" t="s">
         <v>6</v>
       </c>
@@ -1129,13 +1144,13 @@
       <c r="E16" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F16" s="16" t="s">
+      <c r="F16" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="G16" s="16"/>
+      <c r="G16" s="32"/>
     </row>
     <row r="17" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="19"/>
+      <c r="A17" s="31"/>
       <c r="B17" s="2" t="s">
         <v>17</v>
       </c>
@@ -1143,20 +1158,20 @@
       <c r="E17" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F17" s="16" t="s">
+      <c r="F17" s="32" t="s">
         <v>54</v>
       </c>
-      <c r="G17" s="16"/>
+      <c r="G17" s="32"/>
     </row>
     <row r="18" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="19"/>
+      <c r="A18" s="31"/>
       <c r="B18" s="2" t="s">
         <v>18</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E18" s="19"/>
+      <c r="E18" s="31"/>
       <c r="F18" s="4" t="s">
         <v>6</v>
       </c>
@@ -1165,24 +1180,24 @@
       </c>
     </row>
     <row r="19" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A19" s="19"/>
+      <c r="A19" s="31"/>
       <c r="B19" s="1"/>
       <c r="C19" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E19" s="19"/>
+      <c r="E19" s="31"/>
       <c r="F19" s="10" t="s">
         <v>55</v>
       </c>
       <c r="G19" s="10"/>
     </row>
     <row r="20" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A20" s="19"/>
+      <c r="A20" s="31"/>
       <c r="B20" s="1"/>
       <c r="C20" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="E20" s="19"/>
+      <c r="E20" s="31"/>
       <c r="F20" s="2" t="s">
         <v>56</v>
       </c>
@@ -1191,19 +1206,19 @@
       </c>
     </row>
     <row r="21" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="19"/>
+      <c r="A21" s="31"/>
       <c r="B21" s="1"/>
       <c r="C21" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="E21" s="19"/>
+      <c r="E21" s="31"/>
       <c r="F21" s="2" t="s">
         <v>59</v>
       </c>
       <c r="G21" s="2"/>
     </row>
     <row r="22" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="E22" s="19"/>
+      <c r="E22" s="31"/>
       <c r="F22" s="2" t="s">
         <v>37</v>
       </c>
@@ -1215,77 +1230,77 @@
       <c r="A23" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B23" s="17" t="s">
+      <c r="B23" s="33" t="s">
         <v>41</v>
       </c>
-      <c r="C23" s="18"/>
+      <c r="C23" s="34"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B24" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="C24" s="18"/>
+      <c r="B24" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="C24" s="34"/>
       <c r="E24" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F24" s="16" t="s">
+      <c r="F24" s="32" t="s">
         <v>62</v>
       </c>
-      <c r="G24" s="16"/>
+      <c r="G24" s="32"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B25" s="17" t="s">
+      <c r="B25" s="33" t="s">
         <v>42</v>
       </c>
-      <c r="C25" s="18"/>
+      <c r="C25" s="34"/>
       <c r="E25" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F25" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="G25" s="16"/>
+      <c r="F25" s="32" t="s">
+        <v>6</v>
+      </c>
+      <c r="G25" s="32"/>
     </row>
     <row r="26" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B26" s="16" t="s">
+      <c r="B26" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="C26" s="16"/>
+      <c r="C26" s="32"/>
       <c r="E26" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F26" s="16" t="s">
+      <c r="F26" s="32" t="s">
         <v>61</v>
       </c>
-      <c r="G26" s="16"/>
+      <c r="G26" s="32"/>
     </row>
     <row r="27" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B27" s="17" t="s">
+      <c r="B27" s="33" t="s">
         <v>43</v>
       </c>
-      <c r="C27" s="18"/>
+      <c r="C27" s="34"/>
       <c r="E27" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F27" s="16" t="s">
+      <c r="F27" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="G27" s="16"/>
+      <c r="G27" s="32"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="19"/>
+      <c r="A28" s="31"/>
       <c r="B28" s="4" t="s">
         <v>6</v>
       </c>
@@ -1295,20 +1310,20 @@
       <c r="E28" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F28" s="16" t="s">
+      <c r="F28" s="32" t="s">
         <v>60</v>
       </c>
-      <c r="G28" s="16"/>
+      <c r="G28" s="32"/>
     </row>
     <row r="29" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A29" s="19"/>
+      <c r="A29" s="31"/>
       <c r="B29" s="2" t="s">
         <v>45</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="E29" s="20"/>
+      <c r="E29" s="35"/>
       <c r="F29" s="4" t="s">
         <v>6</v>
       </c>
@@ -1320,7 +1335,7 @@
       <c r="A30" s="7"/>
       <c r="B30" s="8"/>
       <c r="C30" s="8"/>
-      <c r="E30" s="21"/>
+      <c r="E30" s="37"/>
       <c r="F30" s="2" t="s">
         <v>63</v>
       </c>
@@ -1329,14 +1344,14 @@
       </c>
     </row>
     <row r="31" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="E31" s="21"/>
+      <c r="E31" s="37"/>
       <c r="F31" s="2"/>
       <c r="G31" s="2" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="E32" s="22"/>
+      <c r="E32" s="36"/>
       <c r="F32" s="1"/>
       <c r="G32" s="2" t="s">
         <v>66</v>
@@ -1346,46 +1361,46 @@
       <c r="E34" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F34" s="16" t="s">
+      <c r="F34" s="32" t="s">
         <v>82</v>
       </c>
-      <c r="G34" s="16"/>
+      <c r="G34" s="32"/>
     </row>
     <row r="35" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E35" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F35" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="G35" s="16"/>
+      <c r="F35" s="32" t="s">
+        <v>6</v>
+      </c>
+      <c r="G35" s="32"/>
     </row>
     <row r="36" spans="5:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E36" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F36" s="16" t="s">
+      <c r="F36" s="32" t="s">
         <v>67</v>
       </c>
-      <c r="G36" s="16"/>
+      <c r="G36" s="32"/>
     </row>
     <row r="37" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E37" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F37" s="16" t="s">
+      <c r="F37" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="G37" s="16"/>
+      <c r="G37" s="32"/>
     </row>
     <row r="38" spans="5:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E38" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F38" s="16" t="s">
+      <c r="F38" s="32" t="s">
         <v>68</v>
       </c>
-      <c r="G38" s="16"/>
+      <c r="G38" s="32"/>
     </row>
     <row r="39" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E39" s="2"/>
@@ -1416,46 +1431,46 @@
       <c r="E43" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F43" s="16" t="s">
+      <c r="F43" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="G43" s="16"/>
+      <c r="G43" s="32"/>
     </row>
     <row r="44" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E44" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F44" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="G44" s="16"/>
+      <c r="F44" s="32" t="s">
+        <v>6</v>
+      </c>
+      <c r="G44" s="32"/>
     </row>
     <row r="45" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E45" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F45" s="16" t="s">
+      <c r="F45" s="32" t="s">
         <v>27</v>
       </c>
-      <c r="G45" s="16"/>
+      <c r="G45" s="32"/>
     </row>
     <row r="46" spans="5:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E46" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F46" s="16" t="s">
+      <c r="F46" s="32" t="s">
         <v>68</v>
       </c>
-      <c r="G46" s="16"/>
+      <c r="G46" s="32"/>
     </row>
     <row r="47" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E47" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F47" s="16" t="s">
+      <c r="F47" s="32" t="s">
         <v>72</v>
       </c>
-      <c r="G47" s="16"/>
+      <c r="G47" s="32"/>
     </row>
     <row r="48" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E48" s="2"/>
@@ -1479,49 +1494,49 @@
       <c r="E51" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F51" s="16" t="s">
+      <c r="F51" s="32" t="s">
         <v>25</v>
       </c>
-      <c r="G51" s="16"/>
+      <c r="G51" s="32"/>
     </row>
     <row r="52" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E52" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F52" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="G52" s="16"/>
+      <c r="F52" s="32" t="s">
+        <v>6</v>
+      </c>
+      <c r="G52" s="32"/>
     </row>
     <row r="53" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E53" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F53" s="16" t="s">
+      <c r="F53" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="G53" s="16"/>
+      <c r="G53" s="32"/>
     </row>
     <row r="54" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E54" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F54" s="16" t="s">
+      <c r="F54" s="32" t="s">
         <v>32</v>
       </c>
-      <c r="G54" s="16"/>
+      <c r="G54" s="32"/>
     </row>
     <row r="55" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E55" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F55" s="16" t="s">
+      <c r="F55" s="32" t="s">
         <v>73</v>
       </c>
-      <c r="G55" s="16"/>
+      <c r="G55" s="32"/>
     </row>
     <row r="56" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E56" s="20"/>
+      <c r="E56" s="35"/>
       <c r="F56" s="9" t="s">
         <v>6</v>
       </c>
@@ -1530,7 +1545,7 @@
       </c>
     </row>
     <row r="57" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E57" s="22"/>
+      <c r="E57" s="36"/>
       <c r="F57" s="2" t="s">
         <v>74</v>
       </c>
@@ -1542,49 +1557,49 @@
       <c r="E59" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F59" s="16" t="s">
+      <c r="F59" s="32" t="s">
         <v>26</v>
       </c>
-      <c r="G59" s="16"/>
+      <c r="G59" s="32"/>
     </row>
     <row r="60" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E60" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F60" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="G60" s="16"/>
+      <c r="F60" s="32" t="s">
+        <v>6</v>
+      </c>
+      <c r="G60" s="32"/>
     </row>
     <row r="61" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E61" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F61" s="16" t="s">
+      <c r="F61" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="G61" s="16"/>
+      <c r="G61" s="32"/>
     </row>
     <row r="62" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E62" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F62" s="16" t="s">
+      <c r="F62" s="32" t="s">
         <v>73</v>
       </c>
-      <c r="G62" s="16"/>
+      <c r="G62" s="32"/>
     </row>
     <row r="63" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E63" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F63" s="16" t="s">
+      <c r="F63" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="G63" s="16"/>
+      <c r="G63" s="32"/>
     </row>
     <row r="64" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E64" s="19"/>
+      <c r="E64" s="31"/>
       <c r="F64" s="15" t="s">
         <v>6</v>
       </c>
@@ -1593,7 +1608,7 @@
       </c>
     </row>
     <row r="65" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E65" s="19"/>
+      <c r="E65" s="31"/>
       <c r="F65" s="13" t="s">
         <v>75</v>
       </c>
@@ -1602,7 +1617,7 @@
       </c>
     </row>
     <row r="66" spans="5:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="E66" s="19"/>
+      <c r="E66" s="31"/>
       <c r="F66" s="13" t="s">
         <v>36</v>
       </c>
@@ -1611,7 +1626,7 @@
       </c>
     </row>
     <row r="67" spans="5:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="E67" s="19"/>
+      <c r="E67" s="31"/>
       <c r="F67" s="13" t="s">
         <v>37</v>
       </c>
@@ -1626,49 +1641,49 @@
       <c r="E69" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F69" s="17" t="s">
+      <c r="F69" s="33" t="s">
         <v>41</v>
       </c>
-      <c r="G69" s="18"/>
+      <c r="G69" s="34"/>
     </row>
     <row r="70" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E70" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F70" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="G70" s="18"/>
+      <c r="F70" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="G70" s="34"/>
     </row>
     <row r="71" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E71" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F71" s="17" t="s">
+      <c r="F71" s="33" t="s">
         <v>42</v>
       </c>
-      <c r="G71" s="18"/>
+      <c r="G71" s="34"/>
     </row>
     <row r="72" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E72" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F72" s="16" t="s">
+      <c r="F72" s="32" t="s">
         <v>73</v>
       </c>
-      <c r="G72" s="16"/>
+      <c r="G72" s="32"/>
     </row>
     <row r="73" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E73" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="F73" s="17" t="s">
+      <c r="F73" s="33" t="s">
         <v>43</v>
       </c>
-      <c r="G73" s="18"/>
+      <c r="G73" s="34"/>
     </row>
     <row r="74" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E74" s="19"/>
+      <c r="E74" s="31"/>
       <c r="F74" s="4" t="s">
         <v>6</v>
       </c>
@@ -1677,7 +1692,7 @@
       </c>
     </row>
     <row r="75" spans="5:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="E75" s="19"/>
+      <c r="E75" s="31"/>
       <c r="F75" s="2" t="s">
         <v>77</v>
       </c>
@@ -1689,49 +1704,49 @@
       <c r="E77" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F77" s="16" t="s">
+      <c r="F77" s="32" t="s">
         <v>78</v>
       </c>
-      <c r="G77" s="16"/>
+      <c r="G77" s="32"/>
     </row>
     <row r="78" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E78" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F78" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="G78" s="18"/>
+      <c r="F78" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="G78" s="34"/>
     </row>
     <row r="79" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E79" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F79" s="16" t="s">
+      <c r="F79" s="32" t="s">
         <v>79</v>
       </c>
-      <c r="G79" s="16"/>
+      <c r="G79" s="32"/>
     </row>
     <row r="80" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E80" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F80" s="16" t="s">
+      <c r="F80" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="G80" s="16"/>
+      <c r="G80" s="32"/>
     </row>
     <row r="81" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E81" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F81" s="23" t="s">
+      <c r="F81" s="30" t="s">
         <v>80</v>
       </c>
-      <c r="G81" s="23"/>
+      <c r="G81" s="30"/>
     </row>
     <row r="82" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E82" s="19"/>
+      <c r="E82" s="31"/>
       <c r="F82" s="4" t="s">
         <v>6</v>
       </c>
@@ -1740,7 +1755,7 @@
       </c>
     </row>
     <row r="83" spans="5:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="E83" s="19"/>
+      <c r="E83" s="31"/>
       <c r="F83" s="2" t="s">
         <v>81</v>
       </c>
@@ -1749,14 +1764,14 @@
       </c>
     </row>
     <row r="84" spans="5:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="E84" s="19"/>
+      <c r="E84" s="31"/>
       <c r="F84" s="2"/>
       <c r="G84" s="2" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="85" spans="5:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="E85" s="19"/>
+      <c r="E85" s="31"/>
       <c r="F85" s="1"/>
       <c r="G85" s="2" t="s">
         <v>84</v>
@@ -1774,51 +1789,6 @@
     </row>
   </sheetData>
   <mergeCells count="70">
-    <mergeCell ref="F81:G81"/>
-    <mergeCell ref="E82:E85"/>
-    <mergeCell ref="F72:G72"/>
-    <mergeCell ref="F73:G73"/>
-    <mergeCell ref="E74:E75"/>
-    <mergeCell ref="F77:G77"/>
-    <mergeCell ref="F78:G78"/>
-    <mergeCell ref="F69:G69"/>
-    <mergeCell ref="F70:G70"/>
-    <mergeCell ref="F71:G71"/>
-    <mergeCell ref="F79:G79"/>
-    <mergeCell ref="F80:G80"/>
-    <mergeCell ref="F60:G60"/>
-    <mergeCell ref="F61:G61"/>
-    <mergeCell ref="F62:G62"/>
-    <mergeCell ref="F63:G63"/>
-    <mergeCell ref="E64:E67"/>
-    <mergeCell ref="F53:G53"/>
-    <mergeCell ref="F54:G54"/>
-    <mergeCell ref="F55:G55"/>
-    <mergeCell ref="E56:E57"/>
-    <mergeCell ref="F59:G59"/>
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="F28:G28"/>
-    <mergeCell ref="E29:E32"/>
-    <mergeCell ref="F51:G51"/>
-    <mergeCell ref="F52:G52"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="A7:A9"/>
-    <mergeCell ref="E7:E11"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="A16:A21"/>
     <mergeCell ref="B23:C23"/>
     <mergeCell ref="B24:C24"/>
     <mergeCell ref="B26:C26"/>
@@ -1834,6 +1804,29 @@
     <mergeCell ref="F26:G26"/>
     <mergeCell ref="B25:C25"/>
     <mergeCell ref="F27:G27"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="A16:A21"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="A7:A9"/>
+    <mergeCell ref="E7:E11"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="E29:E32"/>
+    <mergeCell ref="F51:G51"/>
+    <mergeCell ref="F52:G52"/>
     <mergeCell ref="F34:G34"/>
     <mergeCell ref="F35:G35"/>
     <mergeCell ref="F36:G36"/>
@@ -1844,6 +1837,28 @@
     <mergeCell ref="F43:G43"/>
     <mergeCell ref="F44:G44"/>
     <mergeCell ref="F45:G45"/>
+    <mergeCell ref="F53:G53"/>
+    <mergeCell ref="F54:G54"/>
+    <mergeCell ref="F55:G55"/>
+    <mergeCell ref="E56:E57"/>
+    <mergeCell ref="F59:G59"/>
+    <mergeCell ref="F60:G60"/>
+    <mergeCell ref="F61:G61"/>
+    <mergeCell ref="F62:G62"/>
+    <mergeCell ref="F63:G63"/>
+    <mergeCell ref="E64:E67"/>
+    <mergeCell ref="F69:G69"/>
+    <mergeCell ref="F70:G70"/>
+    <mergeCell ref="F71:G71"/>
+    <mergeCell ref="F79:G79"/>
+    <mergeCell ref="F80:G80"/>
+    <mergeCell ref="F81:G81"/>
+    <mergeCell ref="E82:E85"/>
+    <mergeCell ref="F72:G72"/>
+    <mergeCell ref="F73:G73"/>
+    <mergeCell ref="E74:E75"/>
+    <mergeCell ref="F77:G77"/>
+    <mergeCell ref="F78:G78"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1853,814 +1868,830 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:G87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="E65" sqref="E65:G71"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" style="26" customWidth="1"/>
-    <col min="2" max="3" width="36.28515625" style="26" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" style="26"/>
-    <col min="5" max="5" width="15.7109375" style="26" customWidth="1"/>
-    <col min="6" max="7" width="36.28515625" style="26" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="26"/>
+    <col min="1" max="1" width="15.7109375" style="17" customWidth="1"/>
+    <col min="2" max="3" width="36.28515625" style="17" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="17"/>
+    <col min="5" max="5" width="15.7109375" style="17" customWidth="1"/>
+    <col min="6" max="7" width="36.28515625" style="17" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="17"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="25"/>
-      <c r="E2" s="24" t="s">
+      <c r="C2" s="40"/>
+      <c r="E2" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="25" t="s">
+      <c r="F2" s="40" t="s">
         <v>21</v>
       </c>
-      <c r="G2" s="25"/>
+      <c r="G2" s="40"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="24" t="s">
+      <c r="A3" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="25" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="25"/>
-      <c r="E3" s="24" t="s">
+      <c r="B3" s="40" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="40"/>
+      <c r="E3" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="25" t="s">
-        <v>6</v>
-      </c>
-      <c r="G3" s="25"/>
+      <c r="F3" s="40" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" s="40"/>
     </row>
     <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="24" t="s">
+      <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="25" t="s">
+      <c r="B4" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="25"/>
-      <c r="E4" s="27" t="s">
+      <c r="C4" s="40"/>
+      <c r="E4" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="25" t="s">
+      <c r="F4" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="G4" s="25"/>
+      <c r="G4" s="40"/>
     </row>
     <row r="5" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="24" t="s">
+      <c r="A5" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="25" t="s">
+      <c r="B5" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="25"/>
-      <c r="E5" s="24" t="s">
+      <c r="C5" s="40"/>
+      <c r="E5" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="25" t="s">
+      <c r="F5" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="G5" s="25"/>
+      <c r="G5" s="40"/>
     </row>
     <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="28" t="s">
+      <c r="A6" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="29" t="s">
+      <c r="B6" s="41" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="30"/>
-      <c r="E6" s="31" t="s">
+      <c r="C6" s="42"/>
+      <c r="E6" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="32" t="s">
+      <c r="F6" s="43" t="s">
         <v>23</v>
       </c>
-      <c r="G6" s="32"/>
+      <c r="G6" s="43"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="27"/>
-      <c r="B7" s="33" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="33" t="s">
+      <c r="A7" s="18"/>
+      <c r="B7" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="34"/>
-      <c r="F7" s="33" t="s">
-        <v>6</v>
-      </c>
-      <c r="G7" s="33" t="s">
+      <c r="E7" s="38"/>
+      <c r="F7" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="G7" s="21" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="27"/>
-      <c r="B8" s="35" t="s">
+      <c r="A8" s="18"/>
+      <c r="B8" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="35" t="s">
+      <c r="C8" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="34"/>
-      <c r="F8" s="28" t="s">
+      <c r="E8" s="38"/>
+      <c r="F8" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="G8" s="28" t="s">
+      <c r="G8" s="19" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="27"/>
-      <c r="B9" s="28" t="s">
+      <c r="A9" s="18"/>
+      <c r="B9" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="28" t="s">
+      <c r="C9" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="E9" s="34"/>
-      <c r="F9" s="28"/>
-      <c r="G9" s="28" t="s">
+      <c r="E9" s="38"/>
+      <c r="F9" s="19"/>
+      <c r="G9" s="19" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="27"/>
-      <c r="B10" s="28" t="s">
+      <c r="A10" s="18"/>
+      <c r="B10" s="19" t="s">
         <v>85</v>
       </c>
-      <c r="C10" s="28"/>
-      <c r="E10" s="34"/>
-      <c r="F10" s="24"/>
-      <c r="G10" s="28" t="s">
+      <c r="C10" s="19"/>
+      <c r="E10" s="38"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="19" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="27"/>
-      <c r="B11" s="28" t="s">
+      <c r="A11" s="18"/>
+      <c r="B11" s="19" t="s">
         <v>86</v>
       </c>
-      <c r="C11" s="28" t="s">
+      <c r="C11" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="E11" s="36"/>
-      <c r="F11" s="37"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="24"/>
     </row>
     <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="27"/>
-      <c r="B12" s="24"/>
-      <c r="C12" s="28" t="s">
+      <c r="A12" s="18"/>
+      <c r="B12" s="16"/>
+      <c r="C12" s="19" t="s">
         <v>88</v>
       </c>
-      <c r="E12" s="36"/>
-      <c r="F12" s="37"/>
-      <c r="G12" s="37"/>
+      <c r="E12" s="23"/>
+      <c r="F12" s="24"/>
+      <c r="G12" s="24"/>
     </row>
     <row r="13" spans="1:7" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="27"/>
-      <c r="B13" s="24"/>
-      <c r="C13" s="38" t="s">
+      <c r="A13" s="18"/>
+      <c r="B13" s="16"/>
+      <c r="C13" s="25" t="s">
         <v>89</v>
       </c>
-      <c r="E13" s="24" t="s">
+      <c r="E13" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="F13" s="25" t="s">
+      <c r="F13" s="40" t="s">
         <v>52</v>
       </c>
-      <c r="G13" s="25"/>
+      <c r="G13" s="40"/>
     </row>
     <row r="14" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="36"/>
-      <c r="B14" s="37"/>
-      <c r="C14" s="39"/>
-      <c r="E14" s="24" t="s">
+      <c r="A14" s="23"/>
+      <c r="B14" s="24"/>
+      <c r="C14" s="26"/>
+      <c r="E14" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="F14" s="25" t="s">
-        <v>6</v>
-      </c>
-      <c r="G14" s="25"/>
+      <c r="F14" s="40" t="s">
+        <v>6</v>
+      </c>
+      <c r="G14" s="40"/>
     </row>
     <row r="15" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="37"/>
-      <c r="B15" s="40"/>
-      <c r="C15" s="40"/>
-      <c r="E15" s="24" t="s">
+      <c r="A15" s="24"/>
+      <c r="B15" s="39"/>
+      <c r="C15" s="39"/>
+      <c r="E15" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="F15" s="25" t="s">
+      <c r="F15" s="40" t="s">
         <v>53</v>
       </c>
-      <c r="G15" s="25"/>
+      <c r="G15" s="40"/>
     </row>
     <row r="16" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="36"/>
-      <c r="B16" s="41"/>
-      <c r="C16" s="41"/>
-      <c r="E16" s="24" t="s">
+      <c r="A16" s="23"/>
+      <c r="B16" s="27"/>
+      <c r="C16" s="27"/>
+      <c r="E16" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="F16" s="25" t="s">
+      <c r="F16" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="G16" s="25"/>
+      <c r="G16" s="40"/>
     </row>
     <row r="17" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="36"/>
-      <c r="B17" s="37"/>
-      <c r="C17" s="37"/>
-      <c r="E17" s="28" t="s">
+      <c r="A17" s="23"/>
+      <c r="B17" s="24"/>
+      <c r="C17" s="24"/>
+      <c r="E17" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="F17" s="25" t="s">
+      <c r="F17" s="40" t="s">
         <v>54</v>
       </c>
-      <c r="G17" s="25"/>
+      <c r="G17" s="40"/>
     </row>
     <row r="18" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="36"/>
-      <c r="B18" s="37"/>
-      <c r="C18" s="37"/>
-      <c r="E18" s="34"/>
-      <c r="F18" s="33" t="s">
-        <v>6</v>
-      </c>
-      <c r="G18" s="33" t="s">
+      <c r="A18" s="23"/>
+      <c r="B18" s="24"/>
+      <c r="C18" s="24"/>
+      <c r="E18" s="38"/>
+      <c r="F18" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="G18" s="21" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="36"/>
-      <c r="B19" s="37"/>
-      <c r="C19" s="37"/>
-      <c r="E19" s="34"/>
-      <c r="F19" s="35" t="s">
+      <c r="A19" s="23"/>
+      <c r="B19" s="24"/>
+      <c r="C19" s="24"/>
+      <c r="E19" s="38"/>
+      <c r="F19" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="G19" s="35"/>
+      <c r="G19" s="22"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="36"/>
-      <c r="B20" s="37"/>
-      <c r="C20" s="37"/>
-      <c r="E20" s="34"/>
-      <c r="F20" s="28" t="s">
+      <c r="A20" s="23"/>
+      <c r="B20" s="24"/>
+      <c r="C20" s="24"/>
+      <c r="E20" s="38"/>
+      <c r="F20" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="G20" s="28" t="s">
+      <c r="G20" s="19" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="36"/>
-      <c r="B21" s="37"/>
-      <c r="C21" s="37"/>
-      <c r="E21" s="34"/>
-      <c r="F21" s="28" t="s">
+      <c r="A21" s="23"/>
+      <c r="B21" s="24"/>
+      <c r="C21" s="24"/>
+      <c r="E21" s="38"/>
+      <c r="F21" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="G21" s="28"/>
+      <c r="G21" s="19"/>
     </row>
     <row r="22" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="E22" s="34"/>
-      <c r="F22" s="28" t="s">
+      <c r="E22" s="38"/>
+      <c r="F22" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="G22" s="28" t="s">
+      <c r="G22" s="19" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="24" t="s">
+      <c r="A23" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="B23" s="29" t="s">
+      <c r="B23" s="41" t="s">
         <v>93</v>
       </c>
-      <c r="C23" s="30"/>
+      <c r="C23" s="42"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="24" t="s">
+      <c r="A24" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="B24" s="29" t="s">
-        <v>6</v>
-      </c>
-      <c r="C24" s="30"/>
-      <c r="E24" s="24" t="s">
+      <c r="B24" s="41" t="s">
+        <v>6</v>
+      </c>
+      <c r="C24" s="42"/>
+      <c r="E24" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="F24" s="25" t="s">
+      <c r="F24" s="40" t="s">
         <v>62</v>
       </c>
-      <c r="G24" s="25"/>
+      <c r="G24" s="40"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="24" t="s">
+      <c r="A25" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="B25" s="29" t="s">
+      <c r="B25" s="41" t="s">
         <v>42</v>
       </c>
-      <c r="C25" s="30"/>
-      <c r="E25" s="24" t="s">
+      <c r="C25" s="42"/>
+      <c r="E25" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="F25" s="25" t="s">
-        <v>6</v>
-      </c>
-      <c r="G25" s="25"/>
+      <c r="F25" s="40" t="s">
+        <v>6</v>
+      </c>
+      <c r="G25" s="40"/>
     </row>
     <row r="26" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="24" t="s">
+      <c r="A26" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="B26" s="25" t="s">
+      <c r="B26" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="C26" s="25"/>
-      <c r="E26" s="24" t="s">
+      <c r="C26" s="40"/>
+      <c r="E26" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="F26" s="25" t="s">
+      <c r="F26" s="40" t="s">
         <v>61</v>
       </c>
-      <c r="G26" s="25"/>
+      <c r="G26" s="40"/>
     </row>
     <row r="27" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="42" t="s">
+      <c r="A27" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="B27" s="29" t="s">
+      <c r="B27" s="41" t="s">
         <v>43</v>
       </c>
-      <c r="C27" s="30"/>
-      <c r="E27" s="24" t="s">
+      <c r="C27" s="42"/>
+      <c r="E27" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="F27" s="25" t="s">
+      <c r="F27" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="G27" s="25"/>
+      <c r="G27" s="40"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="34"/>
-      <c r="B28" s="33" t="s">
-        <v>6</v>
-      </c>
-      <c r="C28" s="33" t="s">
+      <c r="A28" s="38"/>
+      <c r="B28" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="C28" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="E28" s="28" t="s">
+      <c r="E28" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="F28" s="25" t="s">
+      <c r="F28" s="40" t="s">
         <v>60</v>
       </c>
-      <c r="G28" s="25"/>
+      <c r="G28" s="40"/>
     </row>
     <row r="29" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="34"/>
-      <c r="B29" s="28" t="s">
+      <c r="A29" s="38"/>
+      <c r="B29" s="19" t="s">
         <v>90</v>
       </c>
-      <c r="C29" s="28" t="s">
+      <c r="C29" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="E29" s="43"/>
-      <c r="F29" s="33" t="s">
-        <v>6</v>
-      </c>
-      <c r="G29" s="33" t="s">
+      <c r="E29" s="44"/>
+      <c r="F29" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="G29" s="21" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="36"/>
-      <c r="B30" s="39"/>
-      <c r="C30" s="39"/>
-      <c r="E30" s="44"/>
-      <c r="F30" s="28" t="s">
+      <c r="A30" s="23"/>
+      <c r="B30" s="26"/>
+      <c r="C30" s="26"/>
+      <c r="E30" s="45"/>
+      <c r="F30" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="G30" s="28" t="s">
+      <c r="G30" s="19" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="E31" s="44"/>
-      <c r="F31" s="28"/>
-      <c r="G31" s="28" t="s">
+      <c r="A31" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="B31" s="41" t="s">
+        <v>110</v>
+      </c>
+      <c r="C31" s="42"/>
+      <c r="E31" s="45"/>
+      <c r="F31" s="19"/>
+      <c r="G31" s="19" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="E32" s="45"/>
-      <c r="F32" s="24"/>
-      <c r="G32" s="28" t="s">
+      <c r="A32" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="B32" s="41" t="s">
+        <v>6</v>
+      </c>
+      <c r="C32" s="42"/>
+      <c r="E32" s="46"/>
+      <c r="F32" s="16"/>
+      <c r="G32" s="19" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="34" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E34" s="24" t="s">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="B33" s="41" t="s">
+        <v>111</v>
+      </c>
+      <c r="C33" s="42"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B34" s="40" t="s">
+        <v>23</v>
+      </c>
+      <c r="C34" s="40"/>
+      <c r="E34" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="F34" s="25" t="s">
+      <c r="F34" s="40" t="s">
         <v>94</v>
       </c>
-      <c r="G34" s="25"/>
-    </row>
-    <row r="35" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E35" s="24" t="s">
+      <c r="G34" s="40"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="B35" s="41" t="s">
+        <v>112</v>
+      </c>
+      <c r="C35" s="42"/>
+      <c r="E35" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="F35" s="25" t="s">
-        <v>6</v>
-      </c>
-      <c r="G35" s="25"/>
-    </row>
-    <row r="36" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E36" s="24" t="s">
+      <c r="F35" s="40" t="s">
+        <v>6</v>
+      </c>
+      <c r="G35" s="40"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="38"/>
+      <c r="B36" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="C36" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="E36" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="F36" s="25" t="s">
+      <c r="F36" s="40" t="s">
         <v>95</v>
       </c>
-      <c r="G36" s="25"/>
-    </row>
-    <row r="37" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E37" s="24" t="s">
+      <c r="G36" s="40"/>
+    </row>
+    <row r="37" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A37" s="38"/>
+      <c r="B37" s="19" t="s">
+        <v>113</v>
+      </c>
+      <c r="C37" s="19" t="s">
+        <v>114</v>
+      </c>
+      <c r="E37" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="F37" s="25" t="s">
+      <c r="F37" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="G37" s="25"/>
-    </row>
-    <row r="38" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E38" s="28" t="s">
+      <c r="G37" s="40"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E38" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="F38" s="25" t="s">
+      <c r="F38" s="40" t="s">
         <v>96</v>
       </c>
-      <c r="G38" s="25"/>
-    </row>
-    <row r="39" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E39" s="28"/>
-      <c r="F39" s="33" t="s">
-        <v>6</v>
-      </c>
-      <c r="G39" s="33" t="s">
+      <c r="G38" s="40"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E39" s="19"/>
+      <c r="F39" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="G39" s="21" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="40" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E40" s="33"/>
-      <c r="F40" s="28" t="s">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E40" s="21"/>
+      <c r="F40" s="19" t="s">
         <v>107</v>
       </c>
-      <c r="G40" s="28" t="s">
+      <c r="G40" s="19" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="41" spans="5:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="E41" s="33"/>
-      <c r="F41" s="28"/>
-      <c r="G41" s="28" t="s">
+    <row r="41" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="E41" s="21"/>
+      <c r="F41" s="19"/>
+      <c r="G41" s="19" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="43" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E43" s="24" t="s">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E43" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="F43" s="25" t="s">
+      <c r="F43" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="G43" s="25"/>
-    </row>
-    <row r="44" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E44" s="24" t="s">
+      <c r="G43" s="40"/>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E44" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="F44" s="25" t="s">
-        <v>6</v>
-      </c>
-      <c r="G44" s="25"/>
-    </row>
-    <row r="45" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E45" s="24" t="s">
+      <c r="F44" s="40" t="s">
+        <v>6</v>
+      </c>
+      <c r="G44" s="40"/>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E45" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="F45" s="25" t="s">
+      <c r="F45" s="40" t="s">
         <v>27</v>
       </c>
-      <c r="G45" s="25"/>
-    </row>
-    <row r="46" spans="5:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E46" s="24" t="s">
+      <c r="G45" s="40"/>
+    </row>
+    <row r="46" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E46" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="F46" s="25" t="s">
+      <c r="F46" s="40" t="s">
         <v>108</v>
       </c>
-      <c r="G46" s="25"/>
-    </row>
-    <row r="47" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E47" s="28" t="s">
+      <c r="G46" s="40"/>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E47" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="F47" s="25" t="s">
+      <c r="F47" s="40" t="s">
         <v>72</v>
       </c>
-      <c r="G47" s="25"/>
-    </row>
-    <row r="48" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E48" s="28"/>
-      <c r="F48" s="33" t="s">
-        <v>6</v>
-      </c>
-      <c r="G48" s="33" t="s">
+      <c r="G47" s="40"/>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E48" s="19"/>
+      <c r="F48" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="G48" s="21" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="49" spans="5:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="E49" s="28"/>
-      <c r="F49" s="28" t="s">
+      <c r="E49" s="19"/>
+      <c r="F49" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="G49" s="28" t="s">
+      <c r="G49" s="19" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="51" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E51" s="24" t="s">
+      <c r="E51" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="F51" s="25" t="s">
+      <c r="F51" s="40" t="s">
         <v>25</v>
       </c>
-      <c r="G51" s="25"/>
+      <c r="G51" s="40"/>
     </row>
     <row r="52" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E52" s="24" t="s">
+      <c r="E52" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="F52" s="25" t="s">
-        <v>6</v>
-      </c>
-      <c r="G52" s="25"/>
+      <c r="F52" s="40" t="s">
+        <v>6</v>
+      </c>
+      <c r="G52" s="40"/>
     </row>
     <row r="53" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E53" s="24" t="s">
+      <c r="E53" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="F53" s="25" t="s">
+      <c r="F53" s="40" t="s">
         <v>31</v>
       </c>
-      <c r="G53" s="25"/>
+      <c r="G53" s="40"/>
     </row>
     <row r="54" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E54" s="24" t="s">
+      <c r="E54" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="F54" s="25" t="s">
+      <c r="F54" s="40" t="s">
         <v>32</v>
       </c>
-      <c r="G54" s="25"/>
+      <c r="G54" s="40"/>
     </row>
     <row r="55" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E55" s="28" t="s">
+      <c r="E55" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="F55" s="25" t="s">
+      <c r="F55" s="40" t="s">
         <v>73</v>
       </c>
-      <c r="G55" s="25"/>
+      <c r="G55" s="40"/>
     </row>
     <row r="56" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E56" s="34"/>
-      <c r="F56" s="33" t="s">
-        <v>6</v>
-      </c>
-      <c r="G56" s="33" t="s">
+      <c r="E56" s="38"/>
+      <c r="F56" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="G56" s="21" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="57" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E57" s="34"/>
-      <c r="F57" s="28" t="s">
+      <c r="E57" s="38"/>
+      <c r="F57" s="19" t="s">
         <v>74</v>
       </c>
-      <c r="G57" s="28" t="s">
+      <c r="G57" s="19" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="58" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E58" s="34"/>
-      <c r="F58" s="28" t="s">
+      <c r="E58" s="38"/>
+      <c r="F58" s="19" t="s">
         <v>97</v>
       </c>
-      <c r="G58" s="24" t="s">
+      <c r="G58" s="16" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="59" spans="5:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E59" s="34"/>
-      <c r="F59" s="28" t="s">
+      <c r="E59" s="38"/>
+      <c r="F59" s="19" t="s">
         <v>99</v>
       </c>
-      <c r="G59" s="28" t="s">
+      <c r="G59" s="19" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="60" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E60" s="34"/>
-      <c r="F60" s="28" t="s">
+      <c r="E60" s="38"/>
+      <c r="F60" s="19" t="s">
         <v>100</v>
       </c>
-      <c r="G60" s="24"/>
+      <c r="G60" s="16"/>
     </row>
     <row r="61" spans="5:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E61" s="34"/>
-      <c r="F61" s="28" t="s">
+      <c r="E61" s="38"/>
+      <c r="F61" s="19" t="s">
         <v>101</v>
       </c>
-      <c r="G61" s="28" t="s">
+      <c r="G61" s="19" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="62" spans="5:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E62" s="34"/>
-      <c r="F62" s="28"/>
-      <c r="G62" s="28" t="s">
+      <c r="E62" s="38"/>
+      <c r="F62" s="19"/>
+      <c r="G62" s="19" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="63" spans="5:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="E63" s="34"/>
-      <c r="F63" s="24"/>
-      <c r="G63" s="28" t="s">
+      <c r="E63" s="38"/>
+      <c r="F63" s="16"/>
+      <c r="G63" s="19" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="64" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E64" s="36"/>
+      <c r="E64" s="23"/>
     </row>
     <row r="65" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E65" s="24" t="s">
+      <c r="E65" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="F65" s="29" t="s">
+      <c r="F65" s="41" t="s">
         <v>106</v>
       </c>
-      <c r="G65" s="30"/>
+      <c r="G65" s="42"/>
     </row>
     <row r="66" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E66" s="24" t="s">
+      <c r="E66" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="F66" s="29" t="s">
-        <v>6</v>
-      </c>
-      <c r="G66" s="30"/>
+      <c r="F66" s="41" t="s">
+        <v>6</v>
+      </c>
+      <c r="G66" s="42"/>
     </row>
     <row r="67" spans="5:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E67" s="24" t="s">
+      <c r="E67" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="F67" s="29" t="s">
+      <c r="F67" s="41" t="s">
         <v>42</v>
       </c>
-      <c r="G67" s="30"/>
+      <c r="G67" s="42"/>
     </row>
     <row r="68" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E68" s="24" t="s">
+      <c r="E68" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="F68" s="25" t="s">
+      <c r="F68" s="40" t="s">
         <v>73</v>
       </c>
-      <c r="G68" s="25"/>
+      <c r="G68" s="40"/>
     </row>
     <row r="69" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E69" s="42" t="s">
+      <c r="E69" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="F69" s="29" t="s">
+      <c r="F69" s="41" t="s">
         <v>43</v>
       </c>
-      <c r="G69" s="30"/>
+      <c r="G69" s="42"/>
     </row>
     <row r="70" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E70" s="34"/>
-      <c r="F70" s="33" t="s">
-        <v>6</v>
-      </c>
-      <c r="G70" s="33" t="s">
+      <c r="E70" s="38"/>
+      <c r="F70" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="G70" s="21" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="71" spans="5:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E71" s="34"/>
-      <c r="F71" s="28" t="s">
+      <c r="E71" s="38"/>
+      <c r="F71" s="19" t="s">
         <v>109</v>
       </c>
-      <c r="G71" s="28" t="s">
+      <c r="G71" s="19" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="72" spans="5:7" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="77" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E77" s="37"/>
-      <c r="F77" s="40"/>
-      <c r="G77" s="40"/>
+      <c r="E77" s="24"/>
+      <c r="F77" s="39"/>
+      <c r="G77" s="39"/>
     </row>
     <row r="78" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E78" s="37"/>
-      <c r="F78" s="40"/>
-      <c r="G78" s="40"/>
+      <c r="E78" s="24"/>
+      <c r="F78" s="39"/>
+      <c r="G78" s="39"/>
     </row>
     <row r="79" spans="5:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E79" s="37"/>
-      <c r="F79" s="40"/>
-      <c r="G79" s="40"/>
+      <c r="E79" s="24"/>
+      <c r="F79" s="39"/>
+      <c r="G79" s="39"/>
     </row>
     <row r="80" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E80" s="37"/>
-      <c r="F80" s="40"/>
-      <c r="G80" s="40"/>
+      <c r="E80" s="24"/>
+      <c r="F80" s="39"/>
+      <c r="G80" s="39"/>
     </row>
     <row r="81" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E81" s="39"/>
-      <c r="F81" s="40"/>
-      <c r="G81" s="40"/>
+      <c r="E81" s="26"/>
+      <c r="F81" s="39"/>
+      <c r="G81" s="39"/>
     </row>
     <row r="86" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E86" s="36"/>
-      <c r="F86" s="37"/>
-      <c r="G86" s="39"/>
+      <c r="E86" s="23"/>
+      <c r="F86" s="24"/>
+      <c r="G86" s="26"/>
     </row>
     <row r="87" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E87" s="36"/>
-      <c r="F87" s="37"/>
-      <c r="G87" s="46"/>
+      <c r="E87" s="23"/>
+      <c r="F87" s="24"/>
+      <c r="G87" s="29"/>
     </row>
   </sheetData>
-  <mergeCells count="57">
-    <mergeCell ref="E70:E71"/>
-    <mergeCell ref="F77:G77"/>
-    <mergeCell ref="F78:G78"/>
-    <mergeCell ref="F54:G54"/>
-    <mergeCell ref="F55:G55"/>
-    <mergeCell ref="F79:G79"/>
-    <mergeCell ref="F80:G80"/>
-    <mergeCell ref="F81:G81"/>
-    <mergeCell ref="F68:G68"/>
-    <mergeCell ref="F69:G69"/>
-    <mergeCell ref="F37:G37"/>
-    <mergeCell ref="F38:G38"/>
-    <mergeCell ref="F51:G51"/>
-    <mergeCell ref="F52:G52"/>
-    <mergeCell ref="F53:G53"/>
-    <mergeCell ref="F44:G44"/>
-    <mergeCell ref="F45:G45"/>
-    <mergeCell ref="F46:G46"/>
-    <mergeCell ref="F47:G47"/>
-    <mergeCell ref="F25:G25"/>
-    <mergeCell ref="F26:G26"/>
-    <mergeCell ref="F27:G27"/>
-    <mergeCell ref="F28:G28"/>
-    <mergeCell ref="F36:G36"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
+  <mergeCells count="63">
+    <mergeCell ref="A36:A37"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B35:C35"/>
     <mergeCell ref="E7:E10"/>
     <mergeCell ref="E56:E63"/>
     <mergeCell ref="F67:G67"/>
@@ -2677,6 +2708,47 @@
     <mergeCell ref="F24:G24"/>
     <mergeCell ref="F34:G34"/>
     <mergeCell ref="F35:G35"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="F26:G26"/>
+    <mergeCell ref="F27:G27"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="F36:G36"/>
+    <mergeCell ref="F37:G37"/>
+    <mergeCell ref="F38:G38"/>
+    <mergeCell ref="F51:G51"/>
+    <mergeCell ref="F52:G52"/>
+    <mergeCell ref="F53:G53"/>
+    <mergeCell ref="F44:G44"/>
+    <mergeCell ref="F45:G45"/>
+    <mergeCell ref="F46:G46"/>
+    <mergeCell ref="F47:G47"/>
+    <mergeCell ref="F79:G79"/>
+    <mergeCell ref="F80:G80"/>
+    <mergeCell ref="F81:G81"/>
+    <mergeCell ref="F68:G68"/>
+    <mergeCell ref="F69:G69"/>
+    <mergeCell ref="E70:E71"/>
+    <mergeCell ref="F77:G77"/>
+    <mergeCell ref="F78:G78"/>
+    <mergeCell ref="F54:G54"/>
+    <mergeCell ref="F55:G55"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>